<commit_message>
age for aug 1 and feb 1 bdays fixed
</commit_message>
<xml_diff>
--- a/calibration.xlsx
+++ b/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Subramanya.Ganti\Downloads\Sports\football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8D24C5-802F-4058-AECD-AB4BF2B3346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AB83B-EA6C-4596-9302-210F35DF4EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{6C434DF2-B60B-4CE1-A463-56AFF8067F06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C434DF2-B60B-4CE1-A463-56AFF8067F06}"/>
   </bookViews>
   <sheets>
     <sheet name="conversions" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2911" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="864">
   <si>
     <t>index</t>
   </si>
@@ -2628,6 +2628,18 @@
   </si>
   <si>
     <t>Santiago Muñóz</t>
+  </si>
+  <si>
+    <t>Goals%</t>
+  </si>
+  <si>
+    <t>Assist%</t>
+  </si>
+  <si>
+    <t>PKatt%</t>
+  </si>
+  <si>
+    <t>Touch%</t>
   </si>
 </sst>
 </file>
@@ -2666,12 +2678,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3008,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB140EA1-8110-4C01-89FA-8BDE6CB07BE7}">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3023,7 +3038,7 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>701</v>
       </c>
@@ -3052,368 +3067,440 @@
         <v>171</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B2" s="1">
-        <v>0.16809024843152801</v>
+        <v>0.164667197464969</v>
       </c>
       <c r="C2" s="1">
-        <v>0.223655469528552</v>
+        <v>0.217201918284426</v>
       </c>
       <c r="D2" s="1">
-        <v>0.18366790781968101</v>
+        <v>0.17590169000081299</v>
       </c>
       <c r="E2" s="1">
-        <v>0.41220621858287998</v>
+        <v>0.40520447199689302</v>
       </c>
       <c r="F2" s="1">
-        <v>0.21172022590172099</v>
+        <v>0.20668412740338901</v>
       </c>
       <c r="G2" s="1">
-        <v>1.33011903627301E-2</v>
+        <v>1.50451346496912E-2</v>
       </c>
       <c r="H2" s="1">
-        <v>0.329817083713558</v>
+        <v>0.34616988421265399</v>
       </c>
       <c r="I2" s="1">
-        <v>0.244879875911201</v>
+        <v>0.253445077426668</v>
       </c>
       <c r="J2" s="1">
-        <v>0.32110772788270697</v>
+        <v>0.379275369550862</v>
       </c>
       <c r="K2" s="1">
-        <v>0.169083880794963</v>
+        <v>0.20003367860400101</v>
       </c>
       <c r="L2" s="1">
-        <v>0.32137459165427001</v>
+        <v>0.79062889547406201</v>
       </c>
       <c r="M2" s="1">
-        <v>0.157085768014493</v>
+        <v>1.13531966159157E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>7.4817400832479106E-2</v>
+        <v>0.33807672736913902</v>
       </c>
       <c r="O2" s="1">
-        <v>0.20527020711664001</v>
+        <v>0.16600524746682199</v>
       </c>
       <c r="P2" s="1">
-        <v>0.32668300181217103</v>
+        <v>0.29821886500973999</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.513925817800028</v>
+        <v>0.163530412494822</v>
       </c>
       <c r="R2" s="1">
-        <v>0.28563508733609499</v>
+        <v>7.7219274401898894E-2</v>
       </c>
       <c r="S2" s="1">
-        <v>0.171823135704956</v>
+        <v>0.18040985685611699</v>
       </c>
       <c r="T2" s="1">
-        <v>0.24021876815460799</v>
+        <v>0.33161231288762499</v>
       </c>
       <c r="U2" s="1">
-        <v>0.20313390263464401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.64297012785460494</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0.27143847761553203</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0.16739327133915399</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0.23778664902368299</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0.198778444205298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>185</v>
       </c>
       <c r="B3" s="1">
-        <v>0.19138964919189899</v>
+        <v>0.19248803450215099</v>
       </c>
       <c r="C3" s="1">
-        <v>0.14422883133809</v>
+        <v>0.13781615317385201</v>
       </c>
       <c r="D3" s="1">
-        <v>0.24175780742706099</v>
+        <v>0.207963887580392</v>
       </c>
       <c r="E3" s="1">
-        <v>0.53790673965090197</v>
+        <v>0.54650033021872402</v>
       </c>
       <c r="F3" s="1">
-        <v>0.251187035676947</v>
+        <v>0.25109771693949601</v>
       </c>
       <c r="G3" s="1">
-        <v>3.8877607765825301E-2</v>
+        <v>3.9622033037627097E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>0.45781072084636898</v>
+        <v>0.47580567461714901</v>
       </c>
       <c r="I3" s="1">
-        <v>0.29885583244018199</v>
+        <v>0.30249149779601398</v>
       </c>
       <c r="J3" s="1">
-        <v>0.50148219147328199</v>
+        <v>0.37457897197872603</v>
       </c>
       <c r="K3" s="1">
-        <v>0.268861703900108</v>
+        <v>0.23801898638354299</v>
       </c>
       <c r="L3" s="1">
-        <v>0.39462699562426001</v>
+        <v>0.66237808128884701</v>
       </c>
       <c r="M3" s="1">
-        <v>0.112211999840775</v>
+        <v>9.4207665824658105E-3</v>
       </c>
       <c r="N3" s="1">
+        <v>0.50897653006355903</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.27209436159616701</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.37745258477374499</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.125530623063108</v>
+      </c>
+      <c r="R3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="1">
-        <v>0.12558149762221199</v>
-      </c>
-      <c r="P3" s="1">
-        <v>8.4362998658114502E-2</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.62766901095306604</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.461932072565025</v>
-      </c>
       <c r="S3" s="1">
-        <v>2.6234518800760401E-2</v>
+        <v>0.10659888390639501</v>
       </c>
       <c r="T3" s="1">
-        <v>0.35060554546599898</v>
+        <v>9.5900803631832399E-2</v>
       </c>
       <c r="U3" s="1">
-        <v>1.30594692300085</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.69366396987406798</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.45106932379249898</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2.2556717876606801E-2</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.33931273734450401</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>1.2238686902251199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B4" s="1">
-        <v>0.21638769909268199</v>
+        <v>0.20924603761409499</v>
       </c>
       <c r="C4" s="1">
-        <v>0.122244159827223</v>
+        <v>0.119648048114009</v>
       </c>
       <c r="D4" s="1">
-        <v>0.21005856728008901</v>
+        <v>0.20859408180880701</v>
       </c>
       <c r="E4" s="1">
-        <v>0.53907069800356999</v>
+        <v>0.54012388947640499</v>
       </c>
       <c r="F4" s="1">
-        <v>0.28226632605623198</v>
+        <v>0.272598195191805</v>
       </c>
       <c r="G4" s="1">
-        <v>4.1164401444850701E-2</v>
+        <v>4.0676906843209799E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>0.49697459690326301</v>
+        <v>0.50880374107016002</v>
       </c>
       <c r="I4" s="1">
-        <v>0.31361318651901998</v>
+        <v>0.30464349910744398</v>
       </c>
       <c r="J4" s="1">
-        <v>0.48633244958654198</v>
+        <v>0.47683254638237099</v>
       </c>
       <c r="K4" s="1">
+        <v>0.27739159360244597</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1.02013434459466</v>
+      </c>
+      <c r="M4" s="1">
+        <v>9.8408047734070102E-3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.49518670483786398</v>
+      </c>
+      <c r="O4" s="1">
         <v>0</v>
       </c>
-      <c r="L4" s="1">
-        <v>0.15576471896925401</v>
-      </c>
-      <c r="M4" s="1">
-        <v>5.8063395130319899E-3</v>
-      </c>
-      <c r="N4" s="1">
-        <v>5.6954948109527698E-2</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.111357954861556</v>
-      </c>
       <c r="P4" s="1">
+        <v>0.13641152181885899</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2.1013061073826299E-2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>5.2672724350133697E-2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>8.8769204228857507E-2</v>
+      </c>
+      <c r="T4" s="1">
         <v>0</v>
       </c>
-      <c r="Q4" s="1">
-        <v>5.4718997024434897E-2</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.44168025515133302</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.210284128419262</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0.20546804506750199</v>
-      </c>
       <c r="U4" s="1">
-        <v>0.72444425664106804</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.170874922345507</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0.425319816443819</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.209440406217621</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0.198965214903018</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0.66618009473170703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B5" s="1">
-        <v>0.26487959756239798</v>
+        <v>0.25790746541027398</v>
       </c>
       <c r="C5" s="1">
-        <v>0.18488780163414401</v>
+        <v>0.185513970705079</v>
       </c>
       <c r="D5" s="1">
-        <v>0.193934322084964</v>
+        <v>0.18366486073518901</v>
       </c>
       <c r="E5" s="1">
-        <v>0.67544742287985204</v>
+        <v>0.68216320424850496</v>
       </c>
       <c r="F5" s="1">
-        <v>0.333196658814786</v>
+        <v>0.32300188737082602</v>
       </c>
       <c r="G5" s="1">
-        <v>3.7092805284769999E-2</v>
+        <v>3.7556935010021497E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>0.506406792094094</v>
+        <v>0.51955878674268896</v>
       </c>
       <c r="I5" s="1">
-        <v>0.33793436122238302</v>
+        <v>0.32994338167271398</v>
       </c>
       <c r="J5" s="1">
-        <v>0.46919627969566902</v>
+        <v>0.39333507098411002</v>
       </c>
       <c r="K5" s="1">
-        <v>9.5917897311995501E-2</v>
+        <v>0.28450716199328702</v>
       </c>
       <c r="L5" s="1">
-        <v>0.21928092864332099</v>
+        <v>0.82059427329882695</v>
       </c>
       <c r="M5" s="1">
-        <v>0.21003219584597599</v>
+        <v>1.96441672830053E-2</v>
       </c>
       <c r="N5" s="1">
-        <v>8.7684009292019E-2</v>
+        <v>0.48008791353899</v>
       </c>
       <c r="O5" s="1">
-        <v>0.17580698722148</v>
+        <v>0.106882234055029</v>
       </c>
       <c r="P5" s="1">
-        <v>8.1413819484501396E-2</v>
+        <v>0.21051312408668099</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.24106215812198101</v>
+        <v>0.19967981779500499</v>
       </c>
       <c r="R5" s="1">
-        <v>0.18247112528897799</v>
+        <v>9.2380576115702703E-2</v>
       </c>
       <c r="S5" s="1">
-        <v>6.7710127725327696E-2</v>
+        <v>0.157497750863339</v>
       </c>
       <c r="T5" s="1">
-        <v>7.3580629492147002E-3</v>
+        <v>8.9763650263735104E-2</v>
       </c>
       <c r="U5" s="1">
-        <v>0.66992244917275601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.29658804752990697</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0.181650577162349</v>
+      </c>
+      <c r="W5" s="1">
+        <v>5.7651659725749302E-2</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0.58810375111909596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B6" s="1">
-        <v>0.14410677016677501</v>
+        <v>0.145830299387498</v>
       </c>
       <c r="C6" s="1">
-        <v>0.214265614243039</v>
+        <v>0.207743282577418</v>
       </c>
       <c r="D6" s="1">
-        <v>0.17157905339564</v>
+        <v>0.16926909537135301</v>
       </c>
       <c r="E6" s="1">
-        <v>0.506212682780529</v>
+        <v>0.52375376479254199</v>
       </c>
       <c r="F6" s="1">
-        <v>0.18180471091975201</v>
+        <v>0.18146799070167799</v>
       </c>
       <c r="G6" s="1">
-        <v>5.3411247239947097E-3</v>
+        <v>6.2006988333092698E-3</v>
       </c>
       <c r="H6" s="1">
-        <v>0.26286919411913301</v>
+        <v>0.283025120825382</v>
       </c>
       <c r="I6" s="1">
-        <v>0.118705097647576</v>
+        <v>0.113561500952091</v>
       </c>
       <c r="J6" s="1">
-        <v>0.432141118295778</v>
+        <v>0.38712908038109201</v>
       </c>
       <c r="K6" s="1">
-        <v>3.4809520290069097E-2</v>
+        <v>0.24457253479167801</v>
       </c>
       <c r="L6" s="1">
-        <v>0.212392808756518</v>
+        <v>0.70350145175308099</v>
       </c>
       <c r="M6" s="1">
-        <v>0.213331051636865</v>
+        <v>1.7257648998398201E-2</v>
       </c>
       <c r="N6" s="1">
-        <v>0.16017328737751599</v>
+        <v>0.45289417570072898</v>
       </c>
       <c r="O6" s="1">
-        <v>0.125676713400069</v>
+        <v>4.9986101095975399E-2</v>
       </c>
       <c r="P6" s="1">
-        <v>0.337680002818317</v>
+        <v>0.20703343485079401</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.22699961886306</v>
+        <v>0.21657869062681601</v>
       </c>
       <c r="R6" s="1">
-        <v>0.22398410583484901</v>
+        <v>0.16910613447006101</v>
       </c>
       <c r="S6" s="1">
-        <v>0.22499121739991201</v>
+        <v>0.111469402055943</v>
       </c>
       <c r="T6" s="1">
-        <v>0.44236401343251402</v>
+        <v>0.33666199008339098</v>
       </c>
       <c r="U6" s="1">
-        <v>0.43406569918565702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.39258375922457001</v>
+      </c>
+      <c r="V6" s="1">
+        <v>0.21226604148926201</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0.22176034892360599</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0.42830935212863103</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0.45121780970434699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>189</v>
       </c>
@@ -3421,711 +3508,843 @@
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0.46852400020847401</v>
+        <v>0.46268240540572297</v>
       </c>
       <c r="D7" s="1">
-        <v>0.14523086158617901</v>
+        <v>0.135709657210245</v>
       </c>
       <c r="E7" s="1">
-        <v>0.13769705607077801</v>
+        <v>0.12532326053963999</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>2.1813531451104901E-2</v>
+        <v>2.3086579100799701E-2</v>
       </c>
       <c r="H7" s="1">
-        <v>4.2618101283561999E-2</v>
+        <v>5.4620532585260201E-2</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>9.94542714915293E-2</v>
+        <v>0.35106797701062098</v>
       </c>
       <c r="K7" s="1">
-        <v>0.144423549200699</v>
+        <v>0.148590010946763</v>
       </c>
       <c r="L7" s="1">
-        <v>0.215789579914552</v>
+        <v>0.68664211403178599</v>
       </c>
       <c r="M7" s="1">
-        <v>0.57564112795836098</v>
+        <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>0.213911695612888</v>
+        <v>0.11475017399868</v>
       </c>
       <c r="O7" s="1">
-        <v>0.22875788106193301</v>
+        <v>0.15021346084140999</v>
       </c>
       <c r="P7" s="1">
-        <v>0.35952155196076102</v>
+        <v>0.201768083140798</v>
       </c>
       <c r="Q7" s="1">
-        <v>0.86712694602025298</v>
+        <v>0.62939652749798702</v>
       </c>
       <c r="R7" s="1">
-        <v>0.424351650317079</v>
+        <v>0.20212734478510899</v>
       </c>
       <c r="S7" s="1">
-        <v>3.0134571460528298E-2</v>
+        <v>0.204678531020897</v>
       </c>
       <c r="T7" s="1">
-        <v>0.238285350264306</v>
+        <v>0.361117364905991</v>
       </c>
       <c r="U7" s="1">
-        <v>1.09018701111981</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1.0893274507025501</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.41228016178738203</v>
+      </c>
+      <c r="W7" s="1">
+        <v>3.2219558616814199E-2</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0.25428325403915297</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1.0656804005840701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B8" s="1">
-        <v>0.123935834630874</v>
+        <v>0.12411971754875201</v>
       </c>
       <c r="C8" s="1">
-        <v>0.41569863056041101</v>
+        <v>0.41055408209402899</v>
       </c>
       <c r="D8" s="1">
-        <v>0.14344843151056</v>
+        <v>0.12982640078358401</v>
       </c>
       <c r="E8" s="1">
-        <v>0.246132254828165</v>
+        <v>0.26956901110367898</v>
       </c>
       <c r="F8" s="1">
-        <v>0.143743291856052</v>
+        <v>0.140596425910261</v>
       </c>
       <c r="G8" s="1">
-        <v>1.2611863157025401E-2</v>
+        <v>1.5056295796324899E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>6.1900056099413403E-2</v>
+        <v>9.2687404891335506E-2</v>
       </c>
       <c r="I8" s="1">
-        <v>0.20613424406876599</v>
+        <v>0.20775092846222301</v>
       </c>
       <c r="J8" s="1">
-        <v>0.27725981404446098</v>
+        <v>0.32995147683175902</v>
       </c>
       <c r="K8" s="1">
-        <v>0.18603723448519</v>
+        <v>0.244890611114011</v>
       </c>
       <c r="L8" s="1">
-        <v>0.24590543157582401</v>
+        <v>0.51524894660522202</v>
       </c>
       <c r="M8" s="1">
-        <v>0.58752811164381202</v>
+        <v>1.55826558492567E-2</v>
       </c>
       <c r="N8" s="1">
-        <v>0.16407017890709699</v>
+        <v>0.31180034790529099</v>
       </c>
       <c r="O8" s="1">
-        <v>9.3849102790528896E-2</v>
+        <v>0.22152510820388199</v>
       </c>
       <c r="P8" s="1">
-        <v>0.59595518290824001</v>
+        <v>0.26524741452919898</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.56253143406071804</v>
+        <v>0.587457058160195</v>
       </c>
       <c r="R8" s="1">
+        <v>0.18777494861348301</v>
+      </c>
+      <c r="S8" s="1">
+        <v>8.6946342811810795E-2</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.60492334306559203</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.65035203449342105</v>
+      </c>
+      <c r="V8" s="1">
         <v>0</v>
       </c>
-      <c r="S8" s="1">
-        <v>1.6971443875164E-2</v>
-      </c>
-      <c r="T8" s="1">
-        <v>0</v>
-      </c>
-      <c r="U8" s="1">
-        <v>0.71090095073440696</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W8" s="1">
+        <v>1.40481302709733E-2</v>
+      </c>
+      <c r="X8" s="1">
+        <v>2.11462082201762E-2</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0.651668288013174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B9" s="1">
-        <v>4.9298740874905503E-2</v>
+        <v>3.4699651349003997E-2</v>
       </c>
       <c r="C9" s="1">
-        <v>0.29884261610847801</v>
+        <v>0.29779487560020002</v>
       </c>
       <c r="D9" s="1">
-        <v>0.17579134833882001</v>
+        <v>0.16557393354725999</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>9.20347509386511E-2</v>
+        <v>7.2284837933941901E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>1.75191959638939E-2</v>
+        <v>1.7763897694751798E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>4.2967026607997798E-3</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>7.7181549316827594E-2</v>
+        <v>5.3148920798814003E-2</v>
       </c>
       <c r="J9" s="1">
+        <v>0.24658733891217599</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.18785586408128099</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.40761829456277099</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1.52863536514725E-2</v>
+      </c>
+      <c r="N9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="1">
-        <v>0.14033801720063799</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0.26453230196764399</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0.43350637079501703</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0.13727317229387101</v>
-      </c>
       <c r="O9" s="1">
-        <v>0.17983778527518299</v>
+        <v>0.15434591615197399</v>
       </c>
       <c r="P9" s="1">
-        <v>0.38587062236553399</v>
+        <v>0.26246941546617703</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.58232623563779695</v>
+        <v>0.44592546307167502</v>
       </c>
       <c r="R9" s="1">
-        <v>0.70332412247554199</v>
+        <v>0.13580108921686401</v>
       </c>
       <c r="S9" s="1">
-        <v>0.164010317471076</v>
+        <v>0.15206723599497601</v>
       </c>
       <c r="T9" s="1">
-        <v>0.94941822344296001</v>
+        <v>0.41610667057124201</v>
       </c>
       <c r="U9" s="1">
-        <v>1.68793093598432</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.60742681218230998</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.68887844067337101</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0.157601576973911</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0.92654810928600295</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>1.75410432061856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B10" s="1">
-        <v>5.9979692943696698E-2</v>
+        <v>5.5043167704210597E-2</v>
       </c>
       <c r="C10" s="1">
-        <v>0.426970122571868</v>
+        <v>0.416347544611882</v>
       </c>
       <c r="D10" s="1">
-        <v>0.11237395349484799</v>
+        <v>0.106440613291041</v>
       </c>
       <c r="E10" s="1">
-        <v>5.1629585082940001E-2</v>
+        <v>3.3678074950925702E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>7.4745443682137702E-2</v>
+        <v>6.9558583513097905E-2</v>
       </c>
       <c r="G10" s="1">
-        <v>1.2671328189612601E-2</v>
+        <v>1.50298803740455E-2</v>
       </c>
       <c r="H10" s="1">
+        <v>1.4957401238488899E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.10237413288404</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.22167574166669299</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.12188679621095901</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.65883530583113803</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.94145194039906E-2</v>
+      </c>
+      <c r="N10" s="1">
+        <v>8.2043926349042104E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.314543844346098</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.34044144660750097</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.53127604058754496</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0.143250723271758</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0.138302568157783</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0.50717591490484504</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1.72183723727988</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0.147780185025227</v>
+      </c>
+      <c r="W10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
-        <v>8.99157249351758E-2</v>
-      </c>
-      <c r="J10" s="1">
-        <v>6.0405867539696803E-2</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0.32293255242594898</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0.36666340656760898</v>
-      </c>
-      <c r="M10" s="1">
-        <v>0.54303021390692097</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0.14549114588610501</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0.16431610912344499</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0.53531408892104104</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1.6160969354182699</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0.165602913510767</v>
-      </c>
-      <c r="S10" s="1">
+      <c r="X10" s="1">
+        <v>0.28820648691962802</v>
+      </c>
+      <c r="Y10" s="1">
         <v>0</v>
       </c>
-      <c r="T10" s="1">
-        <v>0.29513027766637701</v>
-      </c>
-      <c r="U10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B11" s="1">
-        <v>0.11026105788408901</v>
+        <v>0.10678788950474</v>
       </c>
       <c r="C11" s="1">
-        <v>0.34132167779185602</v>
+        <v>0.33546254193361702</v>
       </c>
       <c r="D11" s="1">
-        <v>0.19175488824429299</v>
+        <v>0.18080738820804501</v>
       </c>
       <c r="E11" s="1">
-        <v>0.144870537457291</v>
+        <v>0.14975547721967999</v>
       </c>
       <c r="F11" s="1">
-        <v>0.13110656827112199</v>
+        <v>0.12598262228295901</v>
       </c>
       <c r="G11" s="1">
-        <v>2.2808046832485201E-2</v>
+        <v>2.23576211853302E-2</v>
       </c>
       <c r="H11" s="1">
-        <v>9.2602647324736304E-2</v>
+        <v>0.10077774067925201</v>
       </c>
       <c r="I11" s="1">
-        <v>5.5109148642599803E-2</v>
+        <v>4.2925284247142002E-2</v>
       </c>
       <c r="J11" s="1">
-        <v>0.215993638510071</v>
+        <v>0.225430479902582</v>
       </c>
       <c r="K11" s="1">
-        <v>2.5220963712762601E-2</v>
+        <v>0.16927508875042699</v>
       </c>
       <c r="L11" s="1">
+        <v>0.25098103028144397</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1.30127255150123E-5</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.21777288283194399</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4.3600471441967499E-2</v>
+      </c>
+      <c r="P11" s="1">
         <v>0</v>
       </c>
-      <c r="M11" s="1">
-        <v>0.46646633050799802</v>
-      </c>
-      <c r="N11" s="1">
-        <v>3.72995035167034E-2</v>
-      </c>
-      <c r="O11" s="1">
-        <v>7.9595872754913199E-2</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.40146803773273398</v>
-      </c>
       <c r="Q11" s="1">
-        <v>1.36164900487007</v>
+        <v>0.45680866153376498</v>
       </c>
       <c r="R11" s="1">
-        <v>0.27841947570271502</v>
+        <v>3.2987304931007003E-2</v>
       </c>
       <c r="S11" s="1">
-        <v>5.4212819464317299E-3</v>
+        <v>5.0368704214651699E-2</v>
       </c>
       <c r="T11" s="1">
-        <v>0.36256620696269698</v>
+        <v>0.41292524517556201</v>
       </c>
       <c r="U11" s="1">
-        <v>0.82252487103656302</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1.34943396744667</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.26713998539188299</v>
+      </c>
+      <c r="W11" s="1">
+        <v>8.8877842938051097E-3</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0.359415429938858</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0.89929949923373598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B12" s="1">
-        <v>0.14449039542372</v>
+        <v>0.14062270921536801</v>
       </c>
       <c r="C12" s="1">
-        <v>0.25405507268800398</v>
+        <v>0.24938182577788701</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0.35821240204711002</v>
+        <v>0.35890923552562998</v>
       </c>
       <c r="F12" s="1">
-        <v>0.18444770640438601</v>
+        <v>0.17871573683342601</v>
       </c>
       <c r="G12" s="1">
-        <v>1.0383974409115199E-3</v>
+        <v>3.2135613970379899E-3</v>
       </c>
       <c r="H12" s="1">
-        <v>0.26319426277750702</v>
+        <v>0.27709721402271198</v>
       </c>
       <c r="I12" s="1">
-        <v>0.18083857139658099</v>
+        <v>0.177433495677082</v>
       </c>
       <c r="J12" s="1">
-        <v>0.312089108435816</v>
+        <v>0.175377925132297</v>
       </c>
       <c r="K12" s="1">
-        <v>0.140175395754848</v>
+        <v>0.13299866082696499</v>
       </c>
       <c r="L12" s="1">
-        <v>0.248203479444353</v>
+        <v>1.28734010966686</v>
       </c>
       <c r="M12" s="1">
-        <v>0.316834452047556</v>
+        <v>1.23061015482346E-2</v>
       </c>
       <c r="N12" s="1">
-        <v>0.10274653418855099</v>
+        <v>0.32548802722454301</v>
       </c>
       <c r="O12" s="1">
-        <v>0.131319228414117</v>
+        <v>0.14592239136291299</v>
       </c>
       <c r="P12" s="1">
-        <v>0.31606902691640198</v>
+        <v>0.234098120144758</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.58665810415112596</v>
+        <v>0.31952591687338999</v>
       </c>
       <c r="R12" s="1">
-        <v>0.31448319010749498</v>
+        <v>0.10306415962895001</v>
       </c>
       <c r="S12" s="1">
-        <v>0.10943313477807699</v>
+        <v>0.11150241055441</v>
       </c>
       <c r="T12" s="1">
-        <v>0.28315523929484099</v>
+        <v>0.31422688262512799</v>
       </c>
       <c r="U12" s="1">
-        <v>0.75649213439042595</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.66009660364017797</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0.304211343683297</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0.107786189790074</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0.27779647101122801</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0.74701054826407098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B13" s="1">
-        <v>0.14449039542372</v>
+        <v>0.14062270921536801</v>
       </c>
       <c r="C13" s="1">
-        <v>0.25405507268800398</v>
+        <v>0.24938182577788701</v>
       </c>
       <c r="D13" s="1">
-        <v>0.23033616521067601</v>
+        <v>0.217870123618956</v>
       </c>
       <c r="E13" s="1">
-        <v>0.35821240204711002</v>
+        <v>0.35890923552562998</v>
       </c>
       <c r="F13" s="1">
-        <v>0.18444770640438601</v>
+        <v>0.17871573683342601</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0.26319426277750702</v>
+        <v>0.27709721402271198</v>
       </c>
       <c r="I13" s="1">
-        <v>0.18083857139658099</v>
+        <v>0.177433495677082</v>
       </c>
       <c r="J13" s="1">
-        <v>0.312089108435816</v>
+        <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>0.140175395754848</v>
+        <v>2.91139651372028E-2</v>
       </c>
       <c r="L13" s="1">
-        <v>0.248203479444353</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
-        <v>0.316834452047556</v>
+        <v>1.49716033300131E-2</v>
       </c>
       <c r="N13" s="1">
-        <v>0.10274653418855099</v>
+        <v>0.32548802722454301</v>
       </c>
       <c r="O13" s="1">
-        <v>0.131319228414117</v>
+        <v>0.14592239136291299</v>
       </c>
       <c r="P13" s="1">
-        <v>0.31606902691640198</v>
+        <v>0.234098120144758</v>
       </c>
       <c r="Q13" s="1">
-        <v>0.58665810415112596</v>
+        <v>0.31952591687338999</v>
       </c>
       <c r="R13" s="1">
-        <v>0.31448319010749498</v>
+        <v>0.10306415962895001</v>
       </c>
       <c r="S13" s="1">
-        <v>0.10943313477807699</v>
+        <v>0.11150241055441</v>
       </c>
       <c r="T13" s="1">
-        <v>0.28315523929484099</v>
+        <v>0.31422688262512799</v>
       </c>
       <c r="U13" s="1">
-        <v>0.75649213439042595</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.66009660364017797</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.304211343683297</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0.107786189790074</v>
+      </c>
+      <c r="X13" s="1">
+        <v>0.27779647101122801</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>0.74701054826407098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>542</v>
       </c>
       <c r="B14" s="1">
-        <v>0.14449039542372</v>
+        <v>0.14062270921536801</v>
       </c>
       <c r="C14" s="1">
-        <v>0.25405507268800398</v>
+        <v>0.24938182577788701</v>
       </c>
       <c r="D14" s="1">
-        <v>0.15258753668740699</v>
+        <v>0.12734109934544</v>
       </c>
       <c r="E14" s="1">
-        <v>0.35821240204711002</v>
+        <v>0.35890923552562998</v>
       </c>
       <c r="F14" s="1">
-        <v>0.18444770640438601</v>
+        <v>0.17871573683342601</v>
       </c>
       <c r="G14" s="1">
-        <v>5.8991239718616598E-3</v>
+        <v>8.0440101086094798E-3</v>
       </c>
       <c r="H14" s="1">
-        <v>0.26319426277750702</v>
+        <v>0.27709721402271198</v>
       </c>
       <c r="I14" s="1">
-        <v>0.18083857139658099</v>
+        <v>0.177433495677082</v>
       </c>
       <c r="J14" s="1">
-        <v>0.312089108435816</v>
+        <v>0.19645679974645899</v>
       </c>
       <c r="K14" s="1">
-        <v>0.140175395754848</v>
+        <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>0.248203479444353</v>
+        <v>0.50075504608704402</v>
       </c>
       <c r="M14" s="1">
-        <v>0.316834452047556</v>
+        <v>5.5493873373917597E-3</v>
       </c>
       <c r="N14" s="1">
-        <v>0.10274653418855099</v>
+        <v>0.32548802722454301</v>
       </c>
       <c r="O14" s="1">
-        <v>0.131319228414117</v>
+        <v>0.14592239136291299</v>
       </c>
       <c r="P14" s="1">
-        <v>0.31606902691640198</v>
+        <v>0.234098120144758</v>
       </c>
       <c r="Q14" s="1">
-        <v>0.58665810415112596</v>
+        <v>0.31952591687338999</v>
       </c>
       <c r="R14" s="1">
-        <v>0.31448319010749498</v>
+        <v>0.10306415962895001</v>
       </c>
       <c r="S14" s="1">
-        <v>0.10943313477807699</v>
+        <v>0.11150241055441</v>
       </c>
       <c r="T14" s="1">
-        <v>0.28315523929484099</v>
+        <v>0.31422688262512799</v>
       </c>
       <c r="U14" s="1">
-        <v>0.75649213439042595</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.66009660364017797</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0.304211343683297</v>
+      </c>
+      <c r="W14" s="1">
+        <v>0.107786189790074</v>
+      </c>
+      <c r="X14" s="1">
+        <v>0.27779647101122801</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>0.74701054826407098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>702</v>
       </c>
       <c r="B15" s="1">
-        <v>0.26292249930860401</v>
+        <v>0.26165630801588002</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0.226909785598781</v>
+        <v>0.21453380926243501</v>
       </c>
       <c r="E15" s="1">
-        <v>0.65467325729397297</v>
+        <v>0.65377136185123097</v>
       </c>
       <c r="F15" s="1">
-        <v>0.33191977023045099</v>
+        <v>0.32850609747766701</v>
       </c>
       <c r="G15" s="1">
-        <v>2.60230454752228E-2</v>
+        <v>2.5234502701915702E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>0.55593661511159298</v>
+        <v>0.57481168264668303</v>
       </c>
       <c r="I15" s="1">
-        <v>0.33194648649972902</v>
+        <v>0.33080510878459701</v>
       </c>
       <c r="J15" s="1">
-        <v>0.54489956578050702</v>
+        <v>0.43600030461078298</v>
       </c>
       <c r="K15" s="1">
-        <v>5.7259958357004502E-2</v>
+        <v>0.28253992094286801</v>
       </c>
       <c r="L15" s="1">
-        <v>0.222712155579842</v>
+        <v>1.0795756256700999</v>
       </c>
       <c r="M15" s="1">
-        <v>0</v>
+        <v>2.2435640270931499E-2</v>
       </c>
       <c r="N15" s="1">
-        <v>2.8733324365101599E-2</v>
+        <v>0.56062549089103897</v>
       </c>
       <c r="O15" s="1">
-        <v>0</v>
+        <v>6.4071858350242802E-2</v>
       </c>
       <c r="P15" s="1">
-        <v>0.16261074240256601</v>
+        <v>0.20858483411988199</v>
       </c>
       <c r="Q15" s="1">
         <v>0</v>
       </c>
       <c r="R15" s="1">
-        <v>0.30151258640436701</v>
+        <v>3.49161887127298E-2</v>
       </c>
       <c r="S15" s="1">
-        <v>0.207315589242138</v>
+        <v>0</v>
       </c>
       <c r="T15" s="1">
-        <v>0.14628867883538599</v>
+        <v>0.159400865497001</v>
       </c>
       <c r="U15" s="1">
-        <v>0.67530616209577099</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0.30278570641990699</v>
+      </c>
+      <c r="W15" s="1">
+        <v>0.21643722165489199</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0.14786077722525301</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>0.66812602307487701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>704</v>
       </c>
       <c r="B16" s="1">
-        <v>0.16707850799872301</v>
+        <v>0.16420178758104001</v>
       </c>
       <c r="C16" s="1">
-        <v>0.174560252319819</v>
+        <v>0.17029795241622001</v>
       </c>
       <c r="D16" s="1">
-        <v>0.221376855974698</v>
+        <v>0.209814259383728</v>
       </c>
       <c r="E16" s="1">
-        <v>0.45157131894410302</v>
+        <v>0.45179507878800201</v>
       </c>
       <c r="F16" s="1">
-        <v>0.216935693772772</v>
+        <v>0.21332195689522901</v>
       </c>
       <c r="G16" s="1">
-        <v>1.99533988905592E-2</v>
+        <v>2.0349093230160601E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>0.37855894460546002</v>
+        <v>0.39608854861225301</v>
       </c>
       <c r="I16" s="1">
-        <v>0.17284518790460199</v>
+        <v>0.169366062345608</v>
       </c>
       <c r="J16" s="1">
-        <v>0.39511916406700998</v>
+        <v>0.37871042276154998</v>
       </c>
       <c r="K16" s="1">
-        <v>0.13816975190039901</v>
+        <v>0.27263441750637402</v>
       </c>
       <c r="L16" s="1">
-        <v>0.28878218524795701</v>
+        <v>1.0633808567960199</v>
       </c>
       <c r="M16" s="1">
-        <v>0.29340778188713901</v>
+        <v>2.8329976590492099E-2</v>
       </c>
       <c r="N16" s="1">
-        <v>5.80794950408439E-2</v>
+        <v>0.410138348589906</v>
       </c>
       <c r="O16" s="1">
-        <v>8.7365811299571106E-2</v>
+        <v>0.13447229653214299</v>
       </c>
       <c r="P16" s="1">
-        <v>0.340509536045492</v>
+        <v>0.26449994673785998</v>
       </c>
       <c r="Q16" s="1">
-        <v>0.34898877017789598</v>
+        <v>0.28303289654670799</v>
       </c>
       <c r="R16" s="1">
-        <v>0.31822641507433103</v>
+        <v>5.6210341576417001E-2</v>
       </c>
       <c r="S16" s="1">
-        <v>0.129820679127199</v>
+        <v>7.5728807215040994E-2</v>
       </c>
       <c r="T16" s="1">
-        <v>0.17827478907545599</v>
+        <v>0.31664175031307901</v>
       </c>
       <c r="U16" s="1">
-        <v>0.84113725823986796</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.38421527848668602</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0.30930077518351801</v>
+      </c>
+      <c r="W16" s="1">
+        <v>0.12995471340763001</v>
+      </c>
+      <c r="X16" s="1">
+        <v>0.16329863823641699</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>0.77398406985333901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>703</v>
       </c>
       <c r="B17" s="1">
-        <v>0.12004484242218599</v>
+        <v>0.11144766371716699</v>
       </c>
       <c r="C17" s="1">
-        <v>0.28751676881209598</v>
+        <v>0.28090096019607202</v>
       </c>
       <c r="D17" s="1">
-        <v>0.22987387201718301</v>
+        <v>0.21905931302918899</v>
       </c>
       <c r="E17" s="1">
-        <v>0.29934345503744397</v>
+        <v>0.28418213664696801</v>
       </c>
       <c r="F17" s="1">
-        <v>0.14715970713639301</v>
+        <v>0.13820413721418701</v>
       </c>
       <c r="G17" s="1">
-        <v>1.13621462350853E-2</v>
+        <v>1.0430347232857899E-2</v>
       </c>
       <c r="H17" s="1">
-        <v>0.231733961345613</v>
+        <v>0.23495726417395801</v>
       </c>
       <c r="I17" s="1">
-        <v>0.10378073304749599</v>
+        <v>9.6180049324713496E-2</v>
       </c>
       <c r="J17" s="1">
-        <v>0.25376632129835303</v>
+        <v>0.35410137964719302</v>
       </c>
       <c r="K17" s="1">
-        <v>0.239225115233244</v>
+        <v>0.21708260307730501</v>
       </c>
       <c r="L17" s="1">
-        <v>0.31882012827553402</v>
+        <v>0.98680588658847601</v>
       </c>
       <c r="M17" s="1">
-        <v>0.52080058506784099</v>
+        <v>2.8759990595225299E-2</v>
       </c>
       <c r="N17" s="1">
-        <v>0.171216783217018</v>
+        <v>0.25899113184288403</v>
       </c>
       <c r="O17" s="1">
-        <v>0.12973404685599399</v>
+        <v>0.219250187636164</v>
       </c>
       <c r="P17" s="1">
-        <v>0.49750776480375603</v>
+        <v>0.27063489074061903</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.62346042501704602</v>
+        <v>0.49360766690261598</v>
       </c>
       <c r="R17" s="1">
-        <v>0.30114166173635998</v>
+        <v>0.15538742473119199</v>
       </c>
       <c r="S17" s="1">
-        <v>0.16791374094224801</v>
+        <v>9.6694049881516003E-2</v>
       </c>
       <c r="T17" s="1">
-        <v>0.26504014951591898</v>
+        <v>0.452719562826772</v>
       </c>
       <c r="U17" s="1">
-        <v>0.66889732722980899</v>
+        <v>0.58198223990212306</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0.28483797689811402</v>
+      </c>
+      <c r="W17" s="1">
+        <v>0.16326907797019599</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0.24622126588064</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>0.77012573606958401</v>
       </c>
     </row>
   </sheetData>
@@ -8809,7 +9028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6AACCB-05BA-4A6A-9636-114E61AD6CB6}">
   <dimension ref="A1:D577"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>